<commit_message>
update script to generate supplemental tables
</commit_message>
<xml_diff>
--- a/tables/SupplementalTables_Annotation.xlsx
+++ b/tables/SupplementalTables_Annotation.xlsx
@@ -12,26 +12,26 @@
     <sheet name="TableS5_annot" sheetId="3" r:id="rId3"/>
     <sheet name="TableS6_annot" sheetId="4" r:id="rId4"/>
     <sheet name="TableS7_annot" sheetId="5" r:id="rId5"/>
-    <sheet name="TableS8_annot" sheetId="6" r:id="rId6"/>
-    <sheet name="TableS9_annot" sheetId="7" r:id="rId7"/>
-    <sheet name="TableS10_annot" sheetId="8" r:id="rId8"/>
+    <sheet name="TableS9_annot" sheetId="6" r:id="rId6"/>
+    <sheet name="TableS10_annot" sheetId="7" r:id="rId7"/>
+    <sheet name="TableS11_annot" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">TableS10_annot!$A$1:$B$32</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TableS3_annot!$A$1:$B$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">TableS10_annot!$A$1:$B$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">TableS11_annot!$A$1:$B$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TableS3_annot!$A$1:$B$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TableS4_annot!$A$1:$B$23</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TableS5_annot!$A$1:$B$36</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">TableS6_annot!$A$1:$B$18</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">TableS7_annot!$A$1:$B$42</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">TableS8_annot!$A$1:$B$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">TableS9_annot!$A$1:$B$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">TableS7_annot!$A$1:$B$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">TableS9_annot!$A$1:$B$22</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="339">
   <si>
     <t>column</t>
   </si>
@@ -75,12 +75,6 @@
     <t>Number of SNPs after QC (filtering for number of studies &gt;=10, imputation info score &gt;=0.8, minor allele frequency &gt;=0.02, heterogeneity I^2 &lt;=0.8)</t>
   </si>
   <si>
-    <t>lambda_filtered</t>
-  </si>
-  <si>
-    <t>Inflation factor lambda after QC</t>
-  </si>
-  <si>
     <t>region</t>
   </si>
   <si>
@@ -588,45 +582,18 @@
     <t>HGNC (Ensembl) full name of nearest gene that actually has got a full name</t>
   </si>
   <si>
-    <t>Eigen</t>
-  </si>
-  <si>
-    <t>Eigen is a spectral approach to the functional annotation of genetic variants in coding and noncoding regions. Eigen makes use of a variety of functional annotations in both coding and noncoding regions (such as made available by the ENCODE and Roadmap Epigenomics projects), and combines them into one single measure of functional importance. Eigen is an unsupervised approach, and, unlike most existing methods, is not based on any labelled training data. Eigen produces estimates of predictive accuracy for each functional annotation score, and subsequently uses these estimates of accuracy to derive the aggregate functional score for variants of interest as a weighted linear combination of individual annotations. We show that the resulting meta-score has good discriminatory ability using disease associated and putatively benign variants from published studies (for both Mendelian and complex diseases). The Eigen score is particularly useful in prioritizing likely causal variants in a region of interest when it is combined with population-level genetic data in the framework of a hierarchical model. Furthermore, an important advantage of the Eigen score is that it can be easily adapted to a specific tissue or cell type. More information about the Eigen score can be found in the accompanying manuscript: A spectral approach integrating functional genomic annotations for coding and noncoding variants (Iuliana Ionita-Laza, Kenneth McCallum, Bin Xu, Joseph Buxbaum). and possible confounding factors; therefore, Eigen is a more robust approach at this point.</t>
-  </si>
-  <si>
-    <t>EigenPC</t>
-  </si>
-  <si>
-    <t>Eigen-PC performs well across many scenarios, although, as we discuss in the Supplementary Note, it is more sensitive than Eigen to component annotations and possible confounding factors; therefore, Eigen is a more robust approach at this point.</t>
-  </si>
-  <si>
     <t>CADD_scaled</t>
   </si>
   <si>
     <t>PHRED-like (-10*log10(rank/total)) scaled C-score ranking a variant relative to all possible substitutions of the human genome (8.6x10^9). For details see tab 'deleteriousness'.  Like explained above, a scaled C-score of greater or# equal 10 indicates that these are predicted to be the 10% most deleterious substitutions that you can do to the human genome, a score of greater or equal 20 indicates the 1% most deleterious and so on. If you would like to apply a cutoff on deleteriousness, eg to identify potentially pathogenic variants, we would suggest to put a cutoff somewhere between 10 and 20. Maybe at 15, as this also happens to be the median value for all possible canonical splice site changes and non-synonymous variants. However, there is not a natural choice here -- it is always arbitrary. We therefore recommend integrating C-scores with other evidence and to rank your candidates for follow up rather than hard filtering.</t>
   </si>
   <si>
-    <t>DANN</t>
-  </si>
-  <si>
-    <t>DANN score, similar to CADD, but prediction made using a non-linear kernel function instead of a linear.</t>
-  </si>
-  <si>
-    <t>GWAVA_Region</t>
+    <t>regulome_score</t>
   </si>
   <si>
     <t>Deleteriousness / functional variant relevance score</t>
   </si>
   <si>
-    <t>GWAVA_TSS</t>
-  </si>
-  <si>
-    <t>GWAVA_Unmatched</t>
-  </si>
-  <si>
-    <t>regulome_score</t>
-  </si>
-  <si>
     <t>regulome_score_numeric</t>
   </si>
   <si>
@@ -645,28 +612,10 @@
     <t>cis-eQTL genes for which reported eQTL-SNP has specified min R2 with marker in SNP</t>
   </si>
   <si>
-    <t>transgene</t>
-  </si>
-  <si>
-    <t>trans-eQTL genes for which reported eQTL-SNP has specified min R2 with marker in SNP</t>
-  </si>
-  <si>
     <t>coremine_genes</t>
   </si>
   <si>
-    <t>List of all genes reported for marker in SNP in nearest genes, cis-eQTL genes and trans-eQTL genes</t>
-  </si>
-  <si>
-    <t>hgnc4pathway</t>
-  </si>
-  <si>
-    <t>corresponding HGNC names for pathway genes used</t>
-  </si>
-  <si>
-    <t>entrez4pathway</t>
-  </si>
-  <si>
-    <t>Genes used for pathway enrichment actually used</t>
+    <t>List of all genes reported for marker in SNP in nearest genes, and cis-eQTL genes</t>
   </si>
   <si>
     <t>KEGG</t>
@@ -693,36 +642,6 @@
     <t>Analysis for nominally significant enrichment of genes in  nearest genes, cis-eQTL genes and trans-eQTL genes according to pathway enrichment specific settings in GO categories pathways</t>
   </si>
   <si>
-    <t>tissues</t>
-  </si>
-  <si>
-    <t>Analysis for nominally significant enrichment of genes in  nearest genes, cis-eQTL genes and trans-eQTL genes in high expressed genes of several tissues according to pathway enrichment specific settings</t>
-  </si>
-  <si>
-    <t>GWAMA_phenotype</t>
-  </si>
-  <si>
-    <t>gene</t>
-  </si>
-  <si>
-    <t>Analyzed gene expression of GTEx of NEPTUNE</t>
-  </si>
-  <si>
-    <t>tissue</t>
-  </si>
-  <si>
-    <t>Analyzed tissue for gene expression</t>
-  </si>
-  <si>
-    <t>Number of SNPs included in co-localization analysis per region</t>
-  </si>
-  <si>
-    <t>Posterior probability for hypothesis 1: only trait 1 associated (CKDGen)</t>
-  </si>
-  <si>
-    <t>Posterior probability for hypothesis 2: only trait 2 associated (gene expression)</t>
-  </si>
-  <si>
     <t>region according to locus definition (see Table 1)</t>
   </si>
   <si>
@@ -753,10 +672,7 @@
     <t>TRUE/FALSE vector indicating successful replication in HUNT</t>
   </si>
   <si>
-    <t>NStudies_CKDGen</t>
-  </si>
-  <si>
-    <t>number of studies included in CKDGen Meta analysis for eGFR</t>
+    <t>subgroup analyzed in CKDGen (ALL, MALE, or FEMALE)</t>
   </si>
   <si>
     <t>NSamples_CKDGen</t>
@@ -897,136 +813,241 @@
     <t>P-value in looked-up study</t>
   </si>
   <si>
-    <t>eGFR.N</t>
-  </si>
-  <si>
-    <t>Sample size in eGFR ALL</t>
-  </si>
-  <si>
-    <t>eGFR.effect_allele</t>
-  </si>
-  <si>
-    <t>Effect allele in eGFR ALL</t>
-  </si>
-  <si>
-    <t>eGFR.EAF</t>
-  </si>
-  <si>
-    <t>Effect allele frquency in eGFR ALL</t>
-  </si>
-  <si>
-    <t>eGFR.infoScore</t>
-  </si>
-  <si>
-    <t>Weighted imputation info score in eGFR ALL</t>
-  </si>
-  <si>
-    <t>eGFR.I2</t>
-  </si>
-  <si>
-    <t>Heterogeneity I^2 in eGFR ALL</t>
-  </si>
-  <si>
-    <t>eGFR.beta</t>
-  </si>
-  <si>
-    <t>Beta estimate in eGFR ALL</t>
-  </si>
-  <si>
-    <t>eGFR.SE</t>
-  </si>
-  <si>
-    <t>Standard error in eGFR ALL</t>
-  </si>
-  <si>
-    <t>eGFR.P</t>
-  </si>
-  <si>
-    <t>P-value in eGFR ALL</t>
-  </si>
-  <si>
-    <t>eGFR.logP</t>
-  </si>
-  <si>
-    <t>-log10 transformed p-value in eGFR</t>
-  </si>
-  <si>
-    <t>eGFR.invalid_assoc</t>
-  </si>
-  <si>
-    <t>TRUE/FALSE flag indicating validity of SNP for eGFR ALL (F=valid)</t>
-  </si>
-  <si>
-    <t>eGFR.reason_for_exclusion</t>
-  </si>
-  <si>
-    <t>Reason to exclude SNP for eGFR ALL</t>
-  </si>
-  <si>
-    <t>UA.N</t>
-  </si>
-  <si>
-    <t>Sample size in UA ALL</t>
-  </si>
-  <si>
-    <t>UA.effect_allele</t>
-  </si>
-  <si>
-    <t>Effect allele in UA ALL</t>
-  </si>
-  <si>
-    <t>UA.EAF</t>
-  </si>
-  <si>
-    <t>Effect allele frquency in UA ALL</t>
-  </si>
-  <si>
-    <t>UA.infoScore</t>
-  </si>
-  <si>
-    <t>Weighted imputation info score in UA ALL</t>
-  </si>
-  <si>
-    <t>UA.I2</t>
-  </si>
-  <si>
-    <t>Heterogeneity I^2 in UA ALL</t>
-  </si>
-  <si>
-    <t>UA.beta</t>
-  </si>
-  <si>
-    <t>Beta estimate in UA ALL</t>
-  </si>
-  <si>
-    <t>UA.SE</t>
-  </si>
-  <si>
-    <t>Standard error in UA ALL</t>
-  </si>
-  <si>
-    <t>UA.P</t>
-  </si>
-  <si>
-    <t>P-value in UA ALL</t>
-  </si>
-  <si>
-    <t>UA.logP</t>
-  </si>
-  <si>
-    <t>-log10 transformed p-value in UA</t>
-  </si>
-  <si>
-    <t>UA.invalid_assoc</t>
-  </si>
-  <si>
-    <t>TRUE/FALSE flag indicating validity of SNP for UA ALL (F=valid)</t>
-  </si>
-  <si>
-    <t>UA.reason_for_exclusion</t>
-  </si>
-  <si>
-    <t>Reason to exclude SNP for UA ALL</t>
+    <t>OR or BETA</t>
+  </si>
+  <si>
+    <t>Odds ratio, Z-score or beta estimate in looked-up study</t>
+  </si>
+  <si>
+    <t>SNP_replicated</t>
+  </si>
+  <si>
+    <t>TRUE/FALSE flag indicating successful replication in CKDGen</t>
+  </si>
+  <si>
+    <t>CKDGen phenotype used for replication</t>
+  </si>
+  <si>
+    <t>CKDGen_N</t>
+  </si>
+  <si>
+    <t>Sample size in CKDGen</t>
+  </si>
+  <si>
+    <t>CKDGen_EA</t>
+  </si>
+  <si>
+    <t>CKDGen_EAF</t>
+  </si>
+  <si>
+    <t>Effect allele frquency in CKDGen</t>
+  </si>
+  <si>
+    <t>CKDGen_infoScore</t>
+  </si>
+  <si>
+    <t>Weighted imputation info score in CKDGen</t>
+  </si>
+  <si>
+    <t>CKDGen_I2</t>
+  </si>
+  <si>
+    <t>Heterogeneity I^2 in CKDGen</t>
+  </si>
+  <si>
+    <t>CKDGen_beta</t>
+  </si>
+  <si>
+    <t>CKDGen_SE</t>
+  </si>
+  <si>
+    <t>CKDGen_P</t>
+  </si>
+  <si>
+    <t>CKDGen_logP</t>
+  </si>
+  <si>
+    <t>-log10 transformed p-value in CKDGen</t>
+  </si>
+  <si>
+    <t>CKDGen_invalid</t>
+  </si>
+  <si>
+    <t>TRUE/FALSE flag indicating validity of SNP for CKDGen (F=valid)</t>
+  </si>
+  <si>
+    <t>CKDGen_reason</t>
+  </si>
+  <si>
+    <t>Reason to exclude SNP for CKDGen</t>
+  </si>
+  <si>
+    <t>SNP ID in CKDGen</t>
+  </si>
+  <si>
+    <t>MarkerName</t>
+  </si>
+  <si>
+    <t>Chromosome</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Base position (hg19)</t>
+  </si>
+  <si>
+    <t>Effect allele</t>
+  </si>
+  <si>
+    <t>NEA</t>
+  </si>
+  <si>
+    <t>Non-effect allele</t>
+  </si>
+  <si>
+    <t>EAF</t>
+  </si>
+  <si>
+    <t>Effect allele frequency</t>
+  </si>
+  <si>
+    <t>Nsample</t>
+  </si>
+  <si>
+    <t>Ncohort</t>
+  </si>
+  <si>
+    <t>Number of studies in CKDGen</t>
+  </si>
+  <si>
+    <t>Effects</t>
+  </si>
+  <si>
+    <t>Effect direction across cohorts (+ if the effect allele effect was positive, - if negative, 0 if the effect was zero, ? if marker was not available in cohort)</t>
+  </si>
+  <si>
+    <t>beta_0</t>
+  </si>
+  <si>
+    <t>Effect of first PC of meta-regression</t>
+  </si>
+  <si>
+    <t>se_0</t>
+  </si>
+  <si>
+    <t>Standard error of the effect of first PC of meta-regression</t>
+  </si>
+  <si>
+    <t>beta_1</t>
+  </si>
+  <si>
+    <t>Effect of second PC of meta-regression</t>
+  </si>
+  <si>
+    <t>se_1</t>
+  </si>
+  <si>
+    <t>Standard error of the effect of second PC of meta-regression</t>
+  </si>
+  <si>
+    <t>beta_2</t>
+  </si>
+  <si>
+    <t>Effect of third PC of meta-regression</t>
+  </si>
+  <si>
+    <t>se_2</t>
+  </si>
+  <si>
+    <t>Standard error of the effect of third PC of meta-regression</t>
+  </si>
+  <si>
+    <t>beta_3</t>
+  </si>
+  <si>
+    <t>Effect of fourth PC of meta-regression</t>
+  </si>
+  <si>
+    <t>se_3</t>
+  </si>
+  <si>
+    <t>Standard error of the effect of fourth PC of meta-regression</t>
+  </si>
+  <si>
+    <t>chisq_association</t>
+  </si>
+  <si>
+    <t>Chisq value of the association</t>
+  </si>
+  <si>
+    <t>ndf_association</t>
+  </si>
+  <si>
+    <t>Number of degrees of freedom of the association</t>
+  </si>
+  <si>
+    <t>P-value_association</t>
+  </si>
+  <si>
+    <t>P-value of the association</t>
+  </si>
+  <si>
+    <t>chisq_ancestry_het</t>
+  </si>
+  <si>
+    <t>Chisq value of the heterogeneity due to different ancestry</t>
+  </si>
+  <si>
+    <t>ndf_ancestry_het</t>
+  </si>
+  <si>
+    <t>Number of degrees of freedom of the heterogeneity due to different ancestry</t>
+  </si>
+  <si>
+    <t>P-value_ancestry_het</t>
+  </si>
+  <si>
+    <t>P-value of the heterogeneity due to different ancestry</t>
+  </si>
+  <si>
+    <t>chisq_residual_het</t>
+  </si>
+  <si>
+    <t>Chisq value of the residual heterogeneity</t>
+  </si>
+  <si>
+    <t>ndf_residual_het</t>
+  </si>
+  <si>
+    <t>Number of degrees of freedom  of the residual heterogeneity</t>
+  </si>
+  <si>
+    <t>P-value_residual_het</t>
+  </si>
+  <si>
+    <t>Pvalue of the residual heterogeneity</t>
+  </si>
+  <si>
+    <t>lnBF</t>
+  </si>
+  <si>
+    <t>Log of Bayes factor</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Reason why marker was not analysed in MR-MEGA</t>
+  </si>
+  <si>
+    <t>invalid_assoc</t>
+  </si>
+  <si>
+    <t>setting</t>
+  </si>
+  <si>
+    <t>Phenotype used in CKDGen</t>
   </si>
 </sst>
 </file>
@@ -1367,7 +1388,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1432,16 +1453,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:B8"/>
+  <autoFilter ref="A1:B7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1467,178 +1480,178 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1668,282 +1681,282 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1973,34 +1986,34 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2013,98 +2026,98 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2115,7 +2128,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2142,207 +2155,207 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B22" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B25" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B26" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B27" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B28" t="s">
         <v>194</v>
@@ -2350,18 +2363,18 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B29" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
+        <v>197</v>
+      </c>
+      <c r="B30" t="s">
         <v>198</v>
-      </c>
-      <c r="B30" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -2369,209 +2382,24 @@
         <v>199</v>
       </c>
       <c r="B31" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B32" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
         <v>202</v>
       </c>
-      <c r="B33" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>204</v>
-      </c>
-      <c r="B34" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>206</v>
-      </c>
-      <c r="B35" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
-        <v>208</v>
-      </c>
-      <c r="B36" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
-        <v>210</v>
-      </c>
-      <c r="B37" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
-        <v>212</v>
-      </c>
-      <c r="B38" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>214</v>
-      </c>
-      <c r="B39" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
-        <v>216</v>
-      </c>
-      <c r="B40" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
-        <v>218</v>
-      </c>
-      <c r="B41" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
-        <v>220</v>
-      </c>
-      <c r="B42" t="s">
-        <v>221</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B42"/>
+  <autoFilter ref="A1:B32"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>223</v>
-      </c>
-      <c r="B4" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>225</v>
-      </c>
-      <c r="B5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B11"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B22"/>
   <sheetViews>
@@ -2592,174 +2420,383 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>230</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>231</v>
+        <v>204</v>
       </c>
       <c r="B3" t="s">
-        <v>232</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>233</v>
+        <v>206</v>
       </c>
       <c r="B4" t="s">
-        <v>234</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B5" t="s">
-        <v>235</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>236</v>
+        <v>209</v>
       </c>
       <c r="B6" t="s">
-        <v>237</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>238</v>
+        <v>211</v>
       </c>
       <c r="B7" t="s">
-        <v>239</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>240</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="B9" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="B10" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="B11" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
       <c r="B12" t="s">
-        <v>249</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>250</v>
+        <v>222</v>
       </c>
       <c r="B13" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="B14" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>254</v>
+        <v>226</v>
       </c>
       <c r="B15" t="s">
-        <v>255</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
       <c r="B16" t="s">
-        <v>257</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>258</v>
+        <v>230</v>
       </c>
       <c r="B17" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="B18" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="B19" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="B20" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>266</v>
+        <v>238</v>
       </c>
       <c r="B21" t="s">
-        <v>267</v>
+        <v>239</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="B22" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B22"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>252</v>
+      </c>
+      <c r="B7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>256</v>
+      </c>
+      <c r="B9" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>260</v>
+      </c>
+      <c r="B11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>262</v>
+      </c>
+      <c r="B12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>265</v>
+      </c>
+      <c r="B14" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>267</v>
+      </c>
+      <c r="B15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>268</v>
+      </c>
+      <c r="B16" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>270</v>
+      </c>
+      <c r="B17" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>272</v>
+      </c>
+      <c r="B18" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>274</v>
+      </c>
+      <c r="B19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>275</v>
+      </c>
+      <c r="B20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>276</v>
+      </c>
+      <c r="B21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>277</v>
+      </c>
+      <c r="B22" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>279</v>
+      </c>
+      <c r="B23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>281</v>
+      </c>
+      <c r="B24" t="s">
+        <v>282</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B24"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2785,250 +2822,250 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>270</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="B3" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>274</v>
+        <v>285</v>
       </c>
       <c r="B4" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="B5" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>278</v>
+        <v>209</v>
       </c>
       <c r="B6" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="B7" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="B8" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
       <c r="B9" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="B10" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="B11" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="B12" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="B13" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="B14" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="B15" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="B16" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="B17" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="B18" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B19" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="B20" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B21" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="B22" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="B23" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="B24" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="B25" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="B26" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="B27" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="B28" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="B29" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="B30" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="B31" t="s">
-        <v>329</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="B32" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update supplemental tables (tab7 & tab8)
</commit_message>
<xml_diff>
--- a/tables/SupplementalTables_Annotation.xlsx
+++ b/tables/SupplementalTables_Annotation.xlsx
@@ -12,26 +12,28 @@
     <sheet name="TableS5_annot" sheetId="3" r:id="rId3"/>
     <sheet name="TableS6_annot" sheetId="4" r:id="rId4"/>
     <sheet name="TableS7_annot" sheetId="5" r:id="rId5"/>
-    <sheet name="TableS9_annot" sheetId="6" r:id="rId6"/>
-    <sheet name="TableS10_annot" sheetId="7" r:id="rId7"/>
-    <sheet name="TableS11_annot" sheetId="8" r:id="rId8"/>
+    <sheet name="TableS8_annot" sheetId="6" r:id="rId6"/>
+    <sheet name="TableS9_annot" sheetId="7" r:id="rId7"/>
+    <sheet name="TableS10_annot" sheetId="8" r:id="rId8"/>
+    <sheet name="TableS11_annot" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">TableS10_annot!$A$1:$B$24</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">TableS11_annot!$A$1:$B$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">TableS10_annot!$A$1:$B$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">TableS11_annot!$A$1:$B$32</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TableS3_annot!$A$1:$B$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TableS4_annot!$A$1:$B$23</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TableS5_annot!$A$1:$B$36</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">TableS6_annot!$A$1:$B$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">TableS7_annot!$A$1:$B$32</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">TableS9_annot!$A$1:$B$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">TableS8_annot!$A$1:$B$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">TableS9_annot!$A$1:$B$22</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="348">
   <si>
     <t>column</t>
   </si>
@@ -640,6 +642,33 @@
   </si>
   <si>
     <t>Analysis for nominally significant enrichment of genes in  nearest genes, cis-eQTL genes and trans-eQTL genes according to pathway enrichment specific settings in GO categories pathways</t>
+  </si>
+  <si>
+    <t>Genomic cytoband of gene</t>
+  </si>
+  <si>
+    <t>GWAMA_phenotype</t>
+  </si>
+  <si>
+    <t>gene</t>
+  </si>
+  <si>
+    <t>Analyzed gene expression of GTEx or NEPTUNE</t>
+  </si>
+  <si>
+    <t>tissue</t>
+  </si>
+  <si>
+    <t>Analyzed tissue for gene expression</t>
+  </si>
+  <si>
+    <t>Number of SNPs included in co-localization analysis per region</t>
+  </si>
+  <si>
+    <t>Posterior probability for hypothesis 1: only trait 1 associated (CKDGen)</t>
+  </si>
+  <si>
+    <t>Posterior probability for hypothesis 2: only trait 2 associated (gene expression)</t>
   </si>
   <si>
     <t>region according to locus definition (see Table 1)</t>
@@ -2401,6 +2430,119 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B12"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2423,23 +2565,23 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2447,23 +2589,23 @@
         <v>159</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="B6" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2471,119 +2613,119 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="B9" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="B10" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="B11" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="B12" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="B13" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="B14" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="B15" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="B16" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="B17" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="B18" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="B19" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="B20" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="B21" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="B22" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2592,7 +2734,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B24"/>
   <sheetViews>
@@ -2613,90 +2755,90 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="B2" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="B3" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="B4" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="B5" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="B6" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="B7" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="B8" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="B9" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="B10" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="B11" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="B12" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2704,20 +2846,20 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="B14" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="B15" t="s">
         <v>128</v>
@@ -2725,31 +2867,31 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="B16" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="B17" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="B18" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="B19" t="s">
         <v>132</v>
@@ -2757,7 +2899,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="B20" t="s">
         <v>134</v>
@@ -2765,7 +2907,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="B21" t="s">
         <v>136</v>
@@ -2773,26 +2915,26 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="B22" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="B23" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="B24" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -2801,7 +2943,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B32"/>
   <sheetViews>
@@ -2825,247 +2967,247 @@
         <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
       <c r="B3" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="B4" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="B5" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="B6" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="B7" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="B8" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="B9" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="B10" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="B11" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="B12" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="B13" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="B14" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="B15" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="B16" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="B17" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="B18" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="B19" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="B20" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="B21" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="B22" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="B23" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="B24" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="B25" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="B26" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="B27" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="B28" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="B29" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="B30" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="B31" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="B32" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update SupTabs (S5 - update one-sided p-val; S10 - add position hg19; S11 - add locus number)
</commit_message>
<xml_diff>
--- a/tables/SupplementalTables_Annotation.xlsx
+++ b/tables/SupplementalTables_Annotation.xlsx
@@ -9,33 +9,35 @@
   <sheets>
     <sheet name="TableS3_annot" sheetId="1" r:id="rId1"/>
     <sheet name="TableS4_annot" sheetId="2" r:id="rId2"/>
-    <sheet name="TableS5_annot" sheetId="3" r:id="rId3"/>
-    <sheet name="TableS6_annot" sheetId="4" r:id="rId4"/>
-    <sheet name="TableS7_annot" sheetId="5" r:id="rId5"/>
-    <sheet name="TableS8_annot" sheetId="6" r:id="rId6"/>
-    <sheet name="TableS9_annot" sheetId="7" r:id="rId7"/>
-    <sheet name="TableS10_annot" sheetId="8" r:id="rId8"/>
-    <sheet name="TableS11_annot" sheetId="9" r:id="rId9"/>
-    <sheet name="TableS12_annot" sheetId="10" r:id="rId10"/>
+    <sheet name="TableS5_a_annot" sheetId="3" r:id="rId3"/>
+    <sheet name="TableS5_b_annot" sheetId="4" r:id="rId4"/>
+    <sheet name="TableS6_annot" sheetId="5" r:id="rId5"/>
+    <sheet name="TableS7_annot" sheetId="6" r:id="rId6"/>
+    <sheet name="TableS8_annot" sheetId="7" r:id="rId7"/>
+    <sheet name="TableS9_annot" sheetId="8" r:id="rId8"/>
+    <sheet name="TableS10_annot" sheetId="9" r:id="rId9"/>
+    <sheet name="TableS11_annot" sheetId="10" r:id="rId10"/>
+    <sheet name="TableS12_annot" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">TableS10_annot!$A$1:$B$24</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">TableS11_annot!$A$1:$B$32</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">TableS12_annot!$A$1:$B$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">TableS10_annot!$A$1:$B$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">TableS11_annot!$A$1:$B$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">TableS12_annot!$A$1:$B$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TableS3_annot!$A$1:$B$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TableS4_annot!$A$1:$B$23</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TableS5_annot!$A$1:$B$36</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">TableS6_annot!$A$1:$B$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">TableS7_annot!$A$1:$B$34</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">TableS8_annot!$A$1:$B$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">TableS9_annot!$A$1:$B$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TableS5_a_annot!$A$1:$B$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">TableS5_b_annot!$A$1:$B$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">TableS6_annot!$A$1:$B$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">TableS7_annot!$A$1:$B$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">TableS8_annot!$A$1:$B$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">TableS9_annot!$A$1:$B$23</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="344">
   <si>
     <t>column</t>
   </si>
@@ -79,10 +81,10 @@
     <t>Number of SNPs after QC (filtering for number of studies &gt;=10, imputation info score &gt;=0.8, minor allele frequency &gt;=0.02, heterogeneity I^2 &lt;=0.8)</t>
   </si>
   <si>
-    <t>region</t>
-  </si>
-  <si>
-    <t>Number of associated region (1-15: eGFR, 16-22: UA)</t>
+    <t>locus_NR</t>
+  </si>
+  <si>
+    <t>Number of associated loci (1-15: eGFR, 16-22: UA)</t>
   </si>
   <si>
     <t>cytoband</t>
@@ -94,7 +96,7 @@
     <t>indexSNP</t>
   </si>
   <si>
-    <t>SNP with lowest p-value in this region</t>
+    <t>SNP with lowest p-value in this locus</t>
   </si>
   <si>
     <t>bestSetting</t>
@@ -211,193 +213,67 @@
     <t>Summary of co-localization result, using 0.75 as threshold</t>
   </si>
   <si>
-    <t>N_eGFR</t>
-  </si>
-  <si>
-    <t>Sample size in eGFR (using respective best setting)</t>
-  </si>
-  <si>
-    <t>EAF_eGFR</t>
-  </si>
-  <si>
-    <t>Effect allele frequency in eGFR (using respective best setting)</t>
-  </si>
-  <si>
-    <t>beta_eGFR</t>
-  </si>
-  <si>
-    <t>Beta estimate in eGFR (using respective best setting)</t>
-  </si>
-  <si>
-    <t>SE_eGFR</t>
-  </si>
-  <si>
-    <t>Standard error in eGFR (using respective best setting)</t>
-  </si>
-  <si>
-    <t>P_eGFR</t>
-  </si>
-  <si>
-    <t>P-value in eGFR (using respective best setting)</t>
+    <t>Number of associated locus (1-15: eGFR, 16-22: UA)</t>
   </si>
   <si>
     <t>N_BUN</t>
   </si>
   <si>
-    <t>Sample size in BUN (using respective best setting)</t>
+    <t>Sample size in phenotype indicated in column name (using respective best setting)</t>
   </si>
   <si>
     <t>EAF_BUN</t>
   </si>
   <si>
-    <t>Effect allele frequency in BUN (using respective best setting)</t>
+    <t>Effect allele frequency in phenotype indicated in column name (using respective best setting)</t>
   </si>
   <si>
     <t>beta_BUN</t>
   </si>
   <si>
-    <t>Beta estimate in BUN (using respective best setting)</t>
+    <t>Beta estimate in phenotype indicated in column name (using respective best setting)</t>
   </si>
   <si>
     <t>SE_BUN</t>
   </si>
   <si>
-    <t>Standard error in BUN (using respective best setting)</t>
+    <t>Standard error in phenotype indicated in column name (using respective best setting)</t>
   </si>
   <si>
     <t>P_BUN</t>
   </si>
   <si>
-    <t>P-value in BUN (using respective best setting)</t>
+    <t>P-value in phenotype indicated in column name (using respective best setting)</t>
   </si>
   <si>
     <t>P_oneSided_BUN</t>
   </si>
   <si>
-    <t>One-sided p-value in BUN (using respective best setting)</t>
-  </si>
-  <si>
-    <t>check_BUN</t>
-  </si>
-  <si>
-    <t>TRUE/FALSE flag indicating significant nominal association in BUN with discordant effect direction compared to eGFR (using respective best setting)</t>
-  </si>
-  <si>
-    <t>N_CKD</t>
-  </si>
-  <si>
-    <t>Sample size in CKD (using respective best setting)</t>
-  </si>
-  <si>
-    <t>EAF_CKD</t>
-  </si>
-  <si>
-    <t>Effect allele frequency in CKD (using respective best setting)</t>
-  </si>
-  <si>
-    <t>beta_CKD</t>
-  </si>
-  <si>
-    <t>Beta estimate in CKD (using respective best setting)</t>
-  </si>
-  <si>
-    <t>SE_CKD</t>
-  </si>
-  <si>
-    <t>Standard error in CKD (using respective best setting)</t>
-  </si>
-  <si>
-    <t>P_CKD</t>
-  </si>
-  <si>
-    <t>P-value in CKD (using respective best setting)</t>
-  </si>
-  <si>
-    <t>P_oneSided_CKD</t>
-  </si>
-  <si>
-    <t>One-sided p-value in CKD (using respective best setting)</t>
-  </si>
-  <si>
-    <t>check_CKD</t>
-  </si>
-  <si>
-    <t>TRUE/FALSE flag indicating significant nominal association in CKD with discordant effect direction compared to eGFR (using respective best setting)</t>
-  </si>
-  <si>
-    <t>N_UA</t>
-  </si>
-  <si>
-    <t>Sample size in UA (using respective best setting)</t>
-  </si>
-  <si>
-    <t>EAF_UA</t>
-  </si>
-  <si>
-    <t>Effect allele frequency in UA (using respective best setting)</t>
-  </si>
-  <si>
-    <t>beta_UA</t>
-  </si>
-  <si>
-    <t>Beta estimate in UA (using respective best setting)</t>
-  </si>
-  <si>
-    <t>SE_UA</t>
-  </si>
-  <si>
-    <t>Standard error in UA (using respective best setting)</t>
-  </si>
-  <si>
-    <t>P_UA</t>
-  </si>
-  <si>
-    <t>P-value in UA (using respective best setting)</t>
-  </si>
-  <si>
-    <t>N_Gout</t>
-  </si>
-  <si>
-    <t>EAF_Gout</t>
-  </si>
-  <si>
-    <t>Effect allele frequency in Gout (using respective best setting)</t>
-  </si>
-  <si>
-    <t>beta_Gout</t>
-  </si>
-  <si>
-    <t>Beta estimate in Gout (using respective best setting)</t>
-  </si>
-  <si>
-    <t>SE_Gout</t>
-  </si>
-  <si>
-    <t>Standard error in Gout (using respective best setting)</t>
-  </si>
-  <si>
-    <t>P_Gout</t>
-  </si>
-  <si>
-    <t>P-value in Gout (using respective best setting)</t>
-  </si>
-  <si>
-    <t>P_oneSided_Gout</t>
-  </si>
-  <si>
-    <t>One-sided p-value in Gout (using respective best setting)</t>
-  </si>
-  <si>
-    <t>check_Gout</t>
-  </si>
-  <si>
-    <t>TRUE/FALSE flag indicating significant nominal association in Gout compared to UA (using respective best setting)</t>
+    <t>One-sided p-value in phenotype indicated in column name (using respective best setting, not calculated for eGFR and UA)</t>
+  </si>
+  <si>
+    <t>check_BUN_eGFR</t>
+  </si>
+  <si>
+    <t>TRUE/FALSE flag indicating significant nominal association in phenotype indicated in column name with discordant effect direction compared to eGFR (using respective best setting)</t>
+  </si>
+  <si>
+    <t>check_BUN_UA</t>
+  </si>
+  <si>
+    <t>TRUE/FALSE flag indicating significant nominal association in phenotype indicated in column name with concordant effect direction compared to UA (using respective best setting)</t>
+  </si>
+  <si>
+    <t>eGFR_ALL</t>
+  </si>
+  <si>
+    <t>-log10 transformed p-value in phenotype indicated in column name and setting ALL (one-sided p-value for BUN, CKD, UACR, MA, and gout; two-sided for eGFR and UA)</t>
   </si>
   <si>
     <t>size.region</t>
   </si>
   <si>
-    <t>Range of tested region (not necessary centered around the index SNP)</t>
+    <t>Range of tested locus (not necessary centered around the index SNP)</t>
   </si>
   <si>
     <t>CredSetSize</t>
@@ -499,7 +375,7 @@
     <t>CredSet</t>
   </si>
   <si>
-    <t>ID of the credible set</t>
+    <t>ID of the credible set (locus number + independent signal incase of multiple signals at a locus)</t>
   </si>
   <si>
     <t>PostProb</t>
@@ -556,28 +432,28 @@
     <t>Effect allele frquency</t>
   </si>
   <si>
+    <t>nSamples</t>
+  </si>
+  <si>
+    <t>Weighted Imputation info score</t>
+  </si>
+  <si>
     <t>info</t>
   </si>
   <si>
-    <t>Weighted Imputation info score</t>
-  </si>
-  <si>
-    <t>nSamples</t>
-  </si>
-  <si>
     <t>Sample size per SNP</t>
   </si>
   <si>
-    <t>Beta estimate (conditional in case of region 9, 21, and 22 in setting ALL)</t>
-  </si>
-  <si>
-    <t>Standard error (conditional in case of region 9, 21, and 22 in setting ALL)</t>
+    <t>Beta estimate (conditional in case of locus 9, 21, and 22 in setting ALL)</t>
+  </si>
+  <si>
+    <t>Standard error (conditional in case of locus 9, 21, and 22 in setting ALL)</t>
   </si>
   <si>
     <t>logP</t>
   </si>
   <si>
-    <t>-log10 transformed p-value (conditional in case of region 9, 21, and 22 in setting ALL)</t>
+    <t>-log10 transformed p-value (conditional in case of locus 9, 21, and 22 in setting ALL)</t>
   </si>
   <si>
     <t>I2</t>
@@ -682,7 +558,7 @@
     <t>Analyzed tissue for gene expression</t>
   </si>
   <si>
-    <t>Number of SNPs included in co-localization analysis per region</t>
+    <t>Number of SNPs included in co-localization analysis per locus</t>
   </si>
   <si>
     <t>Posterior probability for hypothesis 1: only trait 1 associated (CKDGen)</t>
@@ -841,7 +717,7 @@
     <t>CHR_POS</t>
   </si>
   <si>
-    <t>Base position in looked-up study</t>
+    <t>Base position in looked-up study (hg38)</t>
   </si>
   <si>
     <t>STRONGEST SNP-RISK ALLELE</t>
@@ -872,6 +748,24 @@
   </si>
   <si>
     <t>Odds ratio, Z-score or beta estimate in looked-up study</t>
+  </si>
+  <si>
+    <t>Genomic cytoband of literature SNP</t>
+  </si>
+  <si>
+    <t>pos_hg19</t>
+  </si>
+  <si>
+    <t>Base position in our study (hg19)</t>
+  </si>
+  <si>
+    <t>litCanGene</t>
+  </si>
+  <si>
+    <t>Candidate Gene as reported in GWAS Catalog</t>
+  </si>
+  <si>
+    <t>Corresponding locus number in our analyses</t>
   </si>
   <si>
     <t>SNP_replicated</t>
@@ -1588,6 +1482,287 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>270</v>
+      </c>
+      <c r="B8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>274</v>
+      </c>
+      <c r="B10" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>275</v>
+      </c>
+      <c r="B11" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>277</v>
+      </c>
+      <c r="B12" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>279</v>
+      </c>
+      <c r="B13" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>281</v>
+      </c>
+      <c r="B14" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>283</v>
+      </c>
+      <c r="B15" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>285</v>
+      </c>
+      <c r="B16" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>287</v>
+      </c>
+      <c r="B17" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>289</v>
+      </c>
+      <c r="B18" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>291</v>
+      </c>
+      <c r="B19" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>293</v>
+      </c>
+      <c r="B20" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>295</v>
+      </c>
+      <c r="B21" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>297</v>
+      </c>
+      <c r="B22" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>299</v>
+      </c>
+      <c r="B23" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>301</v>
+      </c>
+      <c r="B24" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>303</v>
+      </c>
+      <c r="B25" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>305</v>
+      </c>
+      <c r="B26" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>307</v>
+      </c>
+      <c r="B27" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>309</v>
+      </c>
+      <c r="B28" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>311</v>
+      </c>
+      <c r="B29" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>313</v>
+      </c>
+      <c r="B30" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>315</v>
+      </c>
+      <c r="B31" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>317</v>
+      </c>
+      <c r="B32" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>318</v>
+      </c>
+      <c r="B33" t="s">
+        <v>319</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B33"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1607,370 +1782,370 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>356</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>309</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>133</v>
       </c>
       <c r="B8" t="s">
-        <v>357</v>
+        <v>321</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>358</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s">
-        <v>359</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>137</v>
       </c>
       <c r="B12" t="s">
-        <v>360</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>181</v>
+        <v>139</v>
       </c>
       <c r="B13" t="s">
-        <v>361</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>311</v>
+        <v>275</v>
       </c>
       <c r="B14" t="s">
-        <v>312</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>313</v>
+        <v>277</v>
       </c>
       <c r="B15" t="s">
-        <v>314</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>315</v>
+        <v>279</v>
       </c>
       <c r="B16" t="s">
-        <v>362</v>
+        <v>326</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>317</v>
+        <v>281</v>
       </c>
       <c r="B17" t="s">
-        <v>363</v>
+        <v>327</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>319</v>
+        <v>283</v>
       </c>
       <c r="B18" t="s">
-        <v>364</v>
+        <v>328</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>321</v>
+        <v>285</v>
       </c>
       <c r="B19" t="s">
-        <v>365</v>
+        <v>329</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>323</v>
+        <v>287</v>
       </c>
       <c r="B20" t="s">
-        <v>366</v>
+        <v>330</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>325</v>
+        <v>289</v>
       </c>
       <c r="B21" t="s">
-        <v>367</v>
+        <v>331</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>327</v>
+        <v>291</v>
       </c>
       <c r="B22" t="s">
-        <v>368</v>
+        <v>332</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>329</v>
+        <v>293</v>
       </c>
       <c r="B23" t="s">
-        <v>369</v>
+        <v>333</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>331</v>
+        <v>295</v>
       </c>
       <c r="B24" t="s">
-        <v>370</v>
+        <v>334</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="B25" t="s">
-        <v>371</v>
+        <v>335</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>335</v>
+        <v>299</v>
       </c>
       <c r="B26" t="s">
-        <v>372</v>
+        <v>336</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
+        <v>301</v>
+      </c>
+      <c r="B27" t="s">
         <v>337</v>
-      </c>
-      <c r="B27" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>339</v>
+        <v>303</v>
       </c>
       <c r="B28" t="s">
-        <v>374</v>
+        <v>338</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>341</v>
+        <v>305</v>
       </c>
       <c r="B29" t="s">
-        <v>375</v>
+        <v>339</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>343</v>
+        <v>307</v>
       </c>
       <c r="B30" t="s">
-        <v>376</v>
+        <v>340</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>345</v>
+        <v>309</v>
       </c>
       <c r="B31" t="s">
-        <v>377</v>
+        <v>341</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>347</v>
+        <v>311</v>
       </c>
       <c r="B32" t="s">
-        <v>378</v>
+        <v>342</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>349</v>
+        <v>313</v>
       </c>
       <c r="B33" t="s">
-        <v>379</v>
+        <v>343</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>183</v>
+        <v>141</v>
       </c>
       <c r="B34" t="s">
-        <v>184</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>185</v>
+        <v>143</v>
       </c>
       <c r="B35" t="s">
-        <v>186</v>
+        <v>144</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>187</v>
+        <v>145</v>
       </c>
       <c r="B36" t="s">
-        <v>188</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>189</v>
+        <v>147</v>
       </c>
       <c r="B37" t="s">
-        <v>190</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>191</v>
+        <v>149</v>
       </c>
       <c r="B38" t="s">
-        <v>192</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>193</v>
+        <v>151</v>
       </c>
       <c r="B39" t="s">
-        <v>192</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>194</v>
+        <v>152</v>
       </c>
       <c r="B40" t="s">
-        <v>192</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>195</v>
+        <v>153</v>
       </c>
       <c r="B41" t="s">
-        <v>196</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>197</v>
+        <v>155</v>
       </c>
       <c r="B42" t="s">
-        <v>198</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>199</v>
+        <v>157</v>
       </c>
       <c r="B43" t="s">
-        <v>200</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>201</v>
+        <v>159</v>
       </c>
       <c r="B44" t="s">
-        <v>202</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>203</v>
+        <v>161</v>
       </c>
       <c r="B45" t="s">
-        <v>204</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>205</v>
+        <v>163</v>
       </c>
       <c r="B46" t="s">
-        <v>206</v>
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>207</v>
+        <v>165</v>
       </c>
       <c r="B47" t="s">
-        <v>208</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2182,7 +2357,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2204,7 +2379,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2233,259 +2408,140 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
         <v>74</v>
       </c>
-      <c r="B14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>82</v>
-      </c>
-      <c r="B18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>84</v>
-      </c>
-      <c r="B19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>90</v>
-      </c>
-      <c r="B22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>92</v>
-      </c>
-      <c r="B23" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>94</v>
-      </c>
-      <c r="B24" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>98</v>
-      </c>
-      <c r="B26" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>100</v>
-      </c>
-      <c r="B27" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>102</v>
-      </c>
-      <c r="B28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>104</v>
-      </c>
-      <c r="B29" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>106</v>
-      </c>
-      <c r="B30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>107</v>
-      </c>
-      <c r="B31" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>109</v>
-      </c>
-      <c r="B32" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>111</v>
-      </c>
-      <c r="B33" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>113</v>
-      </c>
-      <c r="B34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>115</v>
-      </c>
-      <c r="B35" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
-        <v>117</v>
-      </c>
-      <c r="B36" t="s">
-        <v>118</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B36"/>
+  <autoFilter ref="A1:B13"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B6"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B19"/>
   <sheetViews>
@@ -2509,39 +2565,39 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2554,98 +2610,98 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>129</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>133</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>95</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>101</v>
       </c>
       <c r="B16" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="B17" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>147</v>
+        <v>105</v>
       </c>
       <c r="B18" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="B19" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2654,7 +2710,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B34"/>
   <sheetViews>
@@ -2683,258 +2739,258 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>159</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>161</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s">
-        <v>164</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s">
-        <v>166</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>167</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s">
-        <v>168</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>87</v>
       </c>
       <c r="B12" t="s">
-        <v>169</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>170</v>
+        <v>128</v>
       </c>
       <c r="B13" t="s">
-        <v>171</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>89</v>
       </c>
       <c r="B14" t="s">
-        <v>172</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>173</v>
+        <v>131</v>
       </c>
       <c r="B15" t="s">
-        <v>174</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>175</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s">
-        <v>176</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>133</v>
+        <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>177</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>135</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>178</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>179</v>
+        <v>137</v>
       </c>
       <c r="B19" t="s">
-        <v>180</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>139</v>
       </c>
       <c r="B20" t="s">
-        <v>182</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>183</v>
+        <v>141</v>
       </c>
       <c r="B21" t="s">
-        <v>184</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>185</v>
+        <v>143</v>
       </c>
       <c r="B22" t="s">
-        <v>186</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>187</v>
+        <v>145</v>
       </c>
       <c r="B23" t="s">
-        <v>188</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>189</v>
+        <v>147</v>
       </c>
       <c r="B24" t="s">
-        <v>190</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>191</v>
+        <v>149</v>
       </c>
       <c r="B25" t="s">
-        <v>192</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>193</v>
+        <v>151</v>
       </c>
       <c r="B26" t="s">
-        <v>192</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>194</v>
+        <v>152</v>
       </c>
       <c r="B27" t="s">
-        <v>192</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>195</v>
+        <v>153</v>
       </c>
       <c r="B28" t="s">
-        <v>196</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>197</v>
+        <v>155</v>
       </c>
       <c r="B29" t="s">
-        <v>198</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>199</v>
+        <v>157</v>
       </c>
       <c r="B30" t="s">
-        <v>200</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>201</v>
+        <v>159</v>
       </c>
       <c r="B31" t="s">
-        <v>202</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>203</v>
+        <v>161</v>
       </c>
       <c r="B32" t="s">
-        <v>204</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>205</v>
+        <v>163</v>
       </c>
       <c r="B33" t="s">
-        <v>206</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>207</v>
+        <v>165</v>
       </c>
       <c r="B34" t="s">
-        <v>208</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2943,7 +2999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -2975,12 +3031,12 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>209</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -2988,18 +3044,18 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>213</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3007,7 +3063,7 @@
         <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3023,7 +3079,7 @@
         <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>216</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -3031,7 +3087,7 @@
         <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>217</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -3056,7 +3112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B23"/>
   <sheetViews>
@@ -3080,47 +3136,47 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>218</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>177</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>221</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>223</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>224</v>
+        <v>182</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>226</v>
+        <v>184</v>
       </c>
       <c r="B7" t="s">
-        <v>227</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3128,127 +3184,127 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>228</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>229</v>
+        <v>187</v>
       </c>
       <c r="B9" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>231</v>
+        <v>189</v>
       </c>
       <c r="B10" t="s">
-        <v>232</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>233</v>
+        <v>191</v>
       </c>
       <c r="B11" t="s">
-        <v>234</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>235</v>
+        <v>193</v>
       </c>
       <c r="B12" t="s">
-        <v>236</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>237</v>
+        <v>195</v>
       </c>
       <c r="B13" t="s">
-        <v>238</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="B14" t="s">
-        <v>240</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>241</v>
+        <v>199</v>
       </c>
       <c r="B15" t="s">
-        <v>242</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>243</v>
+        <v>201</v>
       </c>
       <c r="B16" t="s">
-        <v>244</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>245</v>
+        <v>203</v>
       </c>
       <c r="B17" t="s">
-        <v>246</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>247</v>
+        <v>205</v>
       </c>
       <c r="B18" t="s">
-        <v>248</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>249</v>
+        <v>207</v>
       </c>
       <c r="B19" t="s">
-        <v>250</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>251</v>
+        <v>209</v>
       </c>
       <c r="B20" t="s">
-        <v>252</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>253</v>
+        <v>211</v>
       </c>
       <c r="B21" t="s">
-        <v>254</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>255</v>
+        <v>213</v>
       </c>
       <c r="B22" t="s">
-        <v>256</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>257</v>
+        <v>215</v>
       </c>
       <c r="B23" t="s">
-        <v>258</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3257,9 +3313,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3278,463 +3334,222 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>259</v>
+        <v>217</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>261</v>
+        <v>219</v>
       </c>
       <c r="B3" t="s">
-        <v>262</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>263</v>
+        <v>221</v>
       </c>
       <c r="B4" t="s">
-        <v>264</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>265</v>
+        <v>223</v>
       </c>
       <c r="B5" t="s">
-        <v>266</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>267</v>
+        <v>225</v>
       </c>
       <c r="B6" t="s">
-        <v>268</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>269</v>
+        <v>227</v>
       </c>
       <c r="B7" t="s">
-        <v>270</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>271</v>
+        <v>229</v>
       </c>
       <c r="B8" t="s">
-        <v>272</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>273</v>
+        <v>231</v>
       </c>
       <c r="B9" t="s">
-        <v>274</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>275</v>
+        <v>233</v>
       </c>
       <c r="B10" t="s">
-        <v>276</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>277</v>
+        <v>235</v>
       </c>
       <c r="B11" t="s">
-        <v>278</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>279</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>280</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>238</v>
       </c>
       <c r="B13" t="s">
-        <v>281</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>282</v>
+        <v>240</v>
       </c>
       <c r="B14" t="s">
-        <v>283</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>284</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>130</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>285</v>
+        <v>243</v>
       </c>
       <c r="B16" t="s">
-        <v>286</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>287</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>288</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>289</v>
+        <v>246</v>
       </c>
       <c r="B18" t="s">
-        <v>290</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>291</v>
+        <v>248</v>
       </c>
       <c r="B19" t="s">
-        <v>134</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>292</v>
+        <v>249</v>
       </c>
       <c r="B20" t="s">
-        <v>136</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>293</v>
+        <v>251</v>
       </c>
       <c r="B21" t="s">
-        <v>138</v>
+        <v>252</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>294</v>
+        <v>253</v>
       </c>
       <c r="B22" t="s">
-        <v>295</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>296</v>
+        <v>255</v>
       </c>
       <c r="B23" t="s">
-        <v>297</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>298</v>
+        <v>256</v>
       </c>
       <c r="B24" t="s">
-        <v>299</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B24"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>301</v>
-      </c>
-      <c r="B3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>302</v>
-      </c>
-      <c r="B4" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>303</v>
-      </c>
-      <c r="B5" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>224</v>
-      </c>
-      <c r="B6" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>306</v>
-      </c>
-      <c r="B7" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>308</v>
-      </c>
-      <c r="B8" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>310</v>
-      </c>
-      <c r="B9" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>311</v>
-      </c>
-      <c r="B10" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>313</v>
-      </c>
-      <c r="B11" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>315</v>
-      </c>
-      <c r="B12" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>317</v>
-      </c>
-      <c r="B13" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>319</v>
-      </c>
-      <c r="B14" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>321</v>
-      </c>
-      <c r="B15" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>323</v>
-      </c>
-      <c r="B16" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>325</v>
-      </c>
-      <c r="B17" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>327</v>
-      </c>
-      <c r="B18" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>329</v>
-      </c>
-      <c r="B19" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>331</v>
-      </c>
-      <c r="B20" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>333</v>
-      </c>
-      <c r="B21" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>335</v>
-      </c>
-      <c r="B22" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>337</v>
-      </c>
-      <c r="B23" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>339</v>
-      </c>
-      <c r="B24" t="s">
-        <v>340</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>341</v>
+        <v>257</v>
       </c>
       <c r="B25" t="s">
-        <v>342</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>343</v>
+        <v>258</v>
       </c>
       <c r="B26" t="s">
-        <v>344</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>345</v>
+        <v>260</v>
       </c>
       <c r="B27" t="s">
-        <v>346</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>347</v>
+        <v>262</v>
       </c>
       <c r="B28" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>349</v>
-      </c>
-      <c r="B29" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>351</v>
-      </c>
-      <c r="B30" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>353</v>
-      </c>
-      <c r="B31" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>354</v>
-      </c>
-      <c r="B32" t="s">
-        <v>355</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B32"/>
+  <autoFilter ref="A1:B28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>